<commit_message>
fix managed text new lines
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elringus\Documents\UnityProjects\NaninovelSpreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB6B46C-EAF6-4B73-ABCA-23FCFE51B297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53618DEF-A6E3-449B-8F80-670B0E03BB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="11145" yWindow="315" windowWidth="29175" windowHeight="20865" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="11490" yWindow="660" windowWidth="29175" windowHeight="20865" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Scripts&gt;Script001" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="216">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="217">
   <x:si>
     <x:t>Template</x:t>
   </x:si>
@@ -418,6 +418,228 @@
   </x:si>
   <x:si>
     <x:t>Donec ligula nulla, pulvinar a ex suscipit, gravida vulputate orci. Maecenas suscipit nisl vel nibh volutpat varius. Vestibulum turpis sapien, fermentum in tempor in, venenatis vel sapien.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Космогоническая гипотеза Шмидта позволяет достаточно просто объяснить эту нестыковку, однако ощущение мира колеблет интеллект. Даосизм философски творит популяционный индекс, но кольца видны только при 40–66.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Кохан</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Её Величество Юко</x:t>
+  </x:si>
+  <x:si>
+    <x:t>k: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>y: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CGGallery.Title: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Confirmation.No: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Confirmation.Yes: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Auto: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Hide: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Load: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Log: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.QuickLoad: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.QuickSave: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Save: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Settings: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Skip: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Tips: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ControlPanel.Title: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExternalScriptsBrowser.Info: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ExternalScriptsBrowser.Title: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>General.Close: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>General.Return: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.ControlPanelTitleButton.ConfirmationMessage: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsFontDropdown.DefaultFontName: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsFontSizeDropdown.Default: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsFontSizeDropdown.ExtraLarge: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsFontSizeDropdown.Large: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsFontSizeDropdown.Small: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption1: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption2: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption3: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption4: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption5: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption6: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsScreenModeDropdown.ExclusiveFullScreen: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsScreenModeDropdown.FullScreenWindow: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsScreenModeDropdown.MaximizedWindow: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsScreenModeDropdown.Windowed: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsSkipModeDropdown.Everything: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameSettingsSkipModeDropdown.ReadOnly: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.GameStateSlot.EmptySlotLabel: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.SaveLoadMenu.DeleteSaveSlotMessage: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Naninovel.UI.SaveLoadMenu.OverwriteSaveSlotMessage: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SaveLoadMenu.Tab.Load: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SaveLoadMenu.Tab.QuickLoad: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SaveLoadMenu.Tab.Save: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.AutoDelay: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Font: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.FontSize: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Graphics: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Language: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.MessageSpeed: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Preview: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.PreviewText: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Resolution: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.ScreenMode: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.SkipMode: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Tab.Basic: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Tab.Sound: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.Tab.Text: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.VoiceLanguage: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.VolumeEffects: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.VolumeMaster: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.VolumeMusic: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SettingsMenu.VolumeVoice: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.CGGallery: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.Continue: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.Exit: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.ExternalScripts: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.NewGame: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.Settings: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TitleMenu.Tips: {0}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VariableInput.Submit: {0}</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">@printer Fullscreen
@@ -481,297 +703,7 @@
 @goto .Start</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">k: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">y: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">CGGallery.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.No: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.Yes: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Auto: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Hide: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Log: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickSave: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Skip: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Info: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Close: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Return: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.ControlPanelTitleButton.ConfirmationMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontDropdown.DefaultFontName: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Default: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.ExtraLarge: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Large: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Small: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption1: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption2: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption3: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption4: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption5: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption6: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.ExclusiveFullScreen: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.FullScreenWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.MaximizedWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.Windowed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.Everything: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.ReadOnly: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameStateSlot.EmptySlotLabel: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.DeleteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.OverwriteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.AutoDelay: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Font: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.FontSize: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Graphics: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Language: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.MessageSpeed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Preview: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.PreviewText: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Resolution: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.ScreenMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.SkipMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Basic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Sound: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Text: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VoiceLanguage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeEffects: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMaster: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMusic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeVoice: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.CGGallery: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Continue: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Exit: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.ExternalScripts: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.NewGame: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">VariableInput.Submit: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Космогоническая гипотеза Шмидта позволяет достаточно просто объяснить эту нестыковку, однако ощущение мира колеблет интеллект. Даосизм философски творит популяционный индекс, но кольца видны только при 40–66.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Кохан</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Её Величество Юко</x:t>
+    <x:t>ВВОД</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">@printer Fullscreen
@@ -835,290 +767,6 @@
 @goto .Start</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">k: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">y: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">CGGallery.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.No: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.Yes: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Auto: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Hide: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Log: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickSave: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Skip: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Info: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Close: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Return: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.ControlPanelTitleButton.ConfirmationMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontDropdown.DefaultFontName: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Default: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.ExtraLarge: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Large: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Small: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption1: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption2: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption3: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption4: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption5: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption6: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.ExclusiveFullScreen: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.FullScreenWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.MaximizedWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.Windowed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.Everything: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.ReadOnly: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameStateSlot.EmptySlotLabel: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.DeleteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.OverwriteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.AutoDelay: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Font: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.FontSize: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Graphics: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Language: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.MessageSpeed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Preview: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.PreviewText: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Resolution: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.ScreenMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.SkipMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Basic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Sound: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Text: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VoiceLanguage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeEffects: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMaster: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMusic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeVoice: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.CGGallery: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Continue: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Exit: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.ExternalScripts: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.NewGame: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">VariableInput.Submit: {0}
-</x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">@printer Fullscreen
 {0}[i]{1}
 </x:t>
@@ -1178,635 +826,6 @@
   <x:si>
     <x:t xml:space="preserve">
 @goto .Start</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">k: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">y: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">CGGallery.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.No: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.Yes: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Auto: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Hide: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Log: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickSave: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Skip: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Info: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Close: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Return: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.ControlPanelTitleButton.ConfirmationMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontDropdown.DefaultFontName: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Default: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.ExtraLarge: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Large: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Small: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption1: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption2: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption3: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption4: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption5: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption6: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.ExclusiveFullScreen: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.FullScreenWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.MaximizedWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.Windowed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.Everything: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.ReadOnly: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameStateSlot.EmptySlotLabel: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.DeleteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.OverwriteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.AutoDelay: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Font: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.FontSize: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Graphics: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Language: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.MessageSpeed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Preview: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.PreviewText: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Resolution: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.ScreenMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.SkipMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Basic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Sound: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Text: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VoiceLanguage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeEffects: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMaster: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMusic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeVoice: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.CGGallery: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Continue: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Exit: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.ExternalScripts: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.NewGame: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">VariableInput.Submit: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">@printer Fullscreen
-{0}[i]{1}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">{0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">@spawn Rain wait:false
-{0}[br][i]{1}[spawn ShakePrinter params:,1 wait:false]{2}[skipInput]
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-# TestLabel
-@resetText
-; Test comment.
-@printer Wide time:0
-k: {0}[i]{1}[br 2]{2}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">@print {0} speed:0.5 default:false
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">@char Kohaku pos:10,50,-1
-@choice {0} pos:10,50
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">@stop
-@despawn Rain wait:false
-y.Default: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-@goto Script002</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"># Start
-{0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-@input i summary:{0} value:{1}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">@stop
-{0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">
-@goto .Start</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">k: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">y: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">CGGallery.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.No: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Confirmation.Yes: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Auto: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Hide: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Log: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.QuickSave: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Skip: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ControlPanel.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Info: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">ExternalScriptsBrowser.Title: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Close: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">General.Return: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.ControlPanelTitleButton.ConfirmationMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontDropdown.DefaultFontName: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Default: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.ExtraLarge: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Large: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsFontSizeDropdown.Small: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption1: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption2: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption3: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption4: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption5: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsGraphicsDropdown.GraphicOption6: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.ExclusiveFullScreen: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.FullScreenWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.MaximizedWindow: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsScreenModeDropdown.Windowed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.Everything: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameSettingsSkipModeDropdown.ReadOnly: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.GameStateSlot.EmptySlotLabel: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.DeleteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Naninovel.UI.SaveLoadMenu.OverwriteSaveSlotMessage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Load: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.QuickLoad: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaveLoadMenu.Tab.Save: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.AutoDelay: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Font: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.FontSize: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Graphics: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Language: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.MessageSpeed: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Preview: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.PreviewText: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Resolution: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.ScreenMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.SkipMode: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Basic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Sound: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.Tab.Text: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VoiceLanguage: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeEffects: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMaster: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeMusic: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SettingsMenu.VolumeVoice: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.CGGallery: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Continue: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Exit: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.ExternalScripts: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.NewGame: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Settings: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">TitleMenu.Tips: {0}
-</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">VariableInput.Submit: {0}
-</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2178,7 +1197,7 @@
     </x:row>
     <x:row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>382</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>3</x:v>
@@ -2206,7 +1225,7 @@
     </x:row>
     <x:row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <x:c r="A4" s="1" t="s">
-        <x:v>383</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
         <x:v>4</x:v>
@@ -2215,12 +1234,12 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D4" s="1" t="s">
-        <x:v>213</x:v>
+        <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>384</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
         <x:v>5</x:v>
@@ -2262,7 +1281,7 @@
     </x:row>
     <x:row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <x:c r="A8" s="1" t="s">
-        <x:v>385</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
         <x:v>6</x:v>
@@ -2304,7 +1323,7 @@
     </x:row>
     <x:row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A11" s="1" t="s">
-        <x:v>386</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
         <x:v>7</x:v>
@@ -2318,7 +1337,7 @@
     </x:row>
     <x:row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A12" s="1" t="s">
-        <x:v>387</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>8</x:v>
@@ -2332,7 +1351,7 @@
     </x:row>
     <x:row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
-        <x:v>388</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
         <x:v>129</x:v>
@@ -2346,7 +1365,7 @@
     </x:row>
     <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A14" s="1" t="s">
-        <x:v>389</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2384,7 +1403,7 @@
     </x:row>
     <x:row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>390</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>29</x:v>
@@ -2398,7 +1417,7 @@
     </x:row>
     <x:row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
-        <x:v>391</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>30</x:v>
@@ -2426,7 +1445,7 @@
     </x:row>
     <x:row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>392</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
         <x:v>32</x:v>
@@ -2440,7 +1459,7 @@
     </x:row>
     <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A6" s="1" t="s">
-        <x:v>393</x:v>
+        <x:v>240</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2452,7 +1471,7 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0300-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:dimension ref="A1:D3"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="D5" sqref="D5"/>
     </x:sheetView>
   </x:sheetViews>
@@ -2475,9 +1494,9 @@
         <x:v>22</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>394</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>41</x:v>
@@ -2486,12 +1505,12 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="D2" s="1" t="s">
-        <x:v>214</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
-        <x:v>395</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>42</x:v>
@@ -2500,7 +1519,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>215</x:v>
+        <x:v>132</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2512,8 +1531,8 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0400-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:dimension ref="A1:D70"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E2" sqref="E2"/>
+    <x:sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <x:selection activeCell="D72" sqref="D72"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2537,7 +1556,7 @@
     </x:row>
     <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>396</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>45</x:v>
@@ -2551,7 +1570,7 @@
     </x:row>
     <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
-        <x:v>397</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>46</x:v>
@@ -2565,7 +1584,7 @@
     </x:row>
     <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A4" s="1" t="s">
-        <x:v>398</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
         <x:v>47</x:v>
@@ -2579,7 +1598,7 @@
     </x:row>
     <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>399</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
         <x:v>48</x:v>
@@ -2593,7 +1612,7 @@
     </x:row>
     <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A6" s="1" t="s">
-        <x:v>400</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B6" s="1" t="s">
         <x:v>49</x:v>
@@ -2607,7 +1626,7 @@
     </x:row>
     <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A7" s="1" t="s">
-        <x:v>401</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
         <x:v>50</x:v>
@@ -2621,7 +1640,7 @@
     </x:row>
     <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A8" s="1" t="s">
-        <x:v>402</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
         <x:v>51</x:v>
@@ -2635,7 +1654,7 @@
     </x:row>
     <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A9" s="1" t="s">
-        <x:v>403</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
         <x:v>52</x:v>
@@ -2649,7 +1668,7 @@
     </x:row>
     <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A10" s="1" t="s">
-        <x:v>404</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
         <x:v>53</x:v>
@@ -2663,7 +1682,7 @@
     </x:row>
     <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A11" s="1" t="s">
-        <x:v>405</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
         <x:v>54</x:v>
@@ -2677,7 +1696,7 @@
     </x:row>
     <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A12" s="1" t="s">
-        <x:v>406</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>55</x:v>
@@ -2691,7 +1710,7 @@
     </x:row>
     <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
-        <x:v>407</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
         <x:v>56</x:v>
@@ -2705,7 +1724,7 @@
     </x:row>
     <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A14" s="1" t="s">
-        <x:v>408</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
         <x:v>57</x:v>
@@ -2719,7 +1738,7 @@
     </x:row>
     <x:row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A15" s="1" t="s">
-        <x:v>409</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
         <x:v>58</x:v>
@@ -2733,7 +1752,7 @@
     </x:row>
     <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A16" s="1" t="s">
-        <x:v>410</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
         <x:v>59</x:v>
@@ -2747,7 +1766,7 @@
     </x:row>
     <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A17" s="1" t="s">
-        <x:v>411</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
         <x:v>60</x:v>
@@ -2761,7 +1780,7 @@
     </x:row>
     <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A18" s="1" t="s">
-        <x:v>412</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
         <x:v>61</x:v>
@@ -2775,7 +1794,7 @@
     </x:row>
     <x:row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A19" s="1" t="s">
-        <x:v>413</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="B19" s="1" t="s">
         <x:v>62</x:v>
@@ -2789,7 +1808,7 @@
     </x:row>
     <x:row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A20" s="1" t="s">
-        <x:v>414</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="B20" s="1" t="s">
         <x:v>63</x:v>
@@ -2803,7 +1822,7 @@
     </x:row>
     <x:row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A21" s="1" t="s">
-        <x:v>415</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B21" s="1" t="s">
         <x:v>64</x:v>
@@ -2817,7 +1836,7 @@
     </x:row>
     <x:row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A22" s="1" t="s">
-        <x:v>416</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B22" s="1" t="s">
         <x:v>64</x:v>
@@ -2831,7 +1850,7 @@
     </x:row>
     <x:row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A23" s="1" t="s">
-        <x:v>417</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B23" s="1" t="s">
         <x:v>65</x:v>
@@ -2845,7 +1864,7 @@
     </x:row>
     <x:row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A24" s="1" t="s">
-        <x:v>418</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B24" s="1" t="s">
         <x:v>66</x:v>
@@ -2859,7 +1878,7 @@
     </x:row>
     <x:row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A25" s="1" t="s">
-        <x:v>419</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="B25" s="1" t="s">
         <x:v>67</x:v>
@@ -2873,7 +1892,7 @@
     </x:row>
     <x:row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A26" s="1" t="s">
-        <x:v>420</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="B26" s="1" t="s">
         <x:v>68</x:v>
@@ -2887,7 +1906,7 @@
     </x:row>
     <x:row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A27" s="1" t="s">
-        <x:v>421</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B27" s="1" t="s">
         <x:v>69</x:v>
@@ -2901,7 +1920,7 @@
     </x:row>
     <x:row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A28" s="1" t="s">
-        <x:v>422</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="B28" s="1" t="s">
         <x:v>70</x:v>
@@ -2915,7 +1934,7 @@
     </x:row>
     <x:row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A29" s="1" t="s">
-        <x:v>423</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="B29" s="1" t="s">
         <x:v>71</x:v>
@@ -2929,7 +1948,7 @@
     </x:row>
     <x:row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A30" s="1" t="s">
-        <x:v>424</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B30" s="1" t="s">
         <x:v>72</x:v>
@@ -2943,7 +1962,7 @@
     </x:row>
     <x:row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A31" s="1" t="s">
-        <x:v>425</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B31" s="1" t="s">
         <x:v>73</x:v>
@@ -2957,7 +1976,7 @@
     </x:row>
     <x:row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A32" s="1" t="s">
-        <x:v>426</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B32" s="1" t="s">
         <x:v>74</x:v>
@@ -2971,7 +1990,7 @@
     </x:row>
     <x:row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A33" s="1" t="s">
-        <x:v>427</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B33" s="1" t="s">
         <x:v>75</x:v>
@@ -2985,7 +2004,7 @@
     </x:row>
     <x:row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A34" s="1" t="s">
-        <x:v>428</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="B34" s="1" t="s">
         <x:v>76</x:v>
@@ -2999,7 +2018,7 @@
     </x:row>
     <x:row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A35" s="1" t="s">
-        <x:v>429</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="B35" s="1" t="s">
         <x:v>77</x:v>
@@ -3013,7 +2032,7 @@
     </x:row>
     <x:row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A36" s="1" t="s">
-        <x:v>430</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="B36" s="1" t="s">
         <x:v>78</x:v>
@@ -3027,7 +2046,7 @@
     </x:row>
     <x:row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A37" s="1" t="s">
-        <x:v>431</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B37" s="1" t="s">
         <x:v>79</x:v>
@@ -3039,9 +2058,9 @@
         <x:v>79</x:v>
       </x:c>
     </x:row>
-    <x:row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <x:row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A38" s="1" t="s">
-        <x:v>432</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B38" s="1" t="s">
         <x:v>80</x:v>
@@ -3053,9 +2072,9 @@
         <x:v>80</x:v>
       </x:c>
     </x:row>
-    <x:row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <x:row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A39" s="1" t="s">
-        <x:v>433</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="B39" s="1" t="s">
         <x:v>81</x:v>
@@ -3067,9 +2086,9 @@
         <x:v>81</x:v>
       </x:c>
     </x:row>
-    <x:row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <x:row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <x:c r="A40" s="1" t="s">
-        <x:v>434</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B40" s="1" t="s">
         <x:v>82</x:v>
@@ -3081,9 +2100,9 @@
         <x:v>82</x:v>
       </x:c>
     </x:row>
-    <x:row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A41" s="1" t="s">
-        <x:v>435</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B41" s="1" t="s">
         <x:v>50</x:v>
@@ -3095,9 +2114,9 @@
         <x:v>50</x:v>
       </x:c>
     </x:row>
-    <x:row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A42" s="1" t="s">
-        <x:v>436</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="B42" s="1" t="s">
         <x:v>83</x:v>
@@ -3109,9 +2128,9 @@
         <x:v>83</x:v>
       </x:c>
     </x:row>
-    <x:row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A43" s="1" t="s">
-        <x:v>437</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B43" s="1" t="s">
         <x:v>54</x:v>
@@ -3123,9 +2142,9 @@
         <x:v>54</x:v>
       </x:c>
     </x:row>
-    <x:row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A44" s="1" t="s">
-        <x:v>438</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B44" s="1" t="s">
         <x:v>84</x:v>
@@ -3137,9 +2156,9 @@
         <x:v>84</x:v>
       </x:c>
     </x:row>
-    <x:row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A45" s="1" t="s">
-        <x:v>439</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B45" s="1" t="s">
         <x:v>85</x:v>
@@ -3151,9 +2170,9 @@
         <x:v>85</x:v>
       </x:c>
     </x:row>
-    <x:row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A46" s="1" t="s">
-        <x:v>440</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="B46" s="1" t="s">
         <x:v>86</x:v>
@@ -3165,9 +2184,9 @@
         <x:v>86</x:v>
       </x:c>
     </x:row>
-    <x:row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A47" s="1" t="s">
-        <x:v>441</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B47" s="1" t="s">
         <x:v>87</x:v>
@@ -3179,9 +2198,9 @@
         <x:v>87</x:v>
       </x:c>
     </x:row>
-    <x:row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A48" s="1" t="s">
-        <x:v>442</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B48" s="1" t="s">
         <x:v>88</x:v>
@@ -3193,9 +2212,9 @@
         <x:v>88</x:v>
       </x:c>
     </x:row>
-    <x:row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A49" s="1" t="s">
-        <x:v>443</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="B49" s="1" t="s">
         <x:v>89</x:v>
@@ -3207,9 +2226,9 @@
         <x:v>89</x:v>
       </x:c>
     </x:row>
-    <x:row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A50" s="1" t="s">
-        <x:v>444</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B50" s="1" t="s">
         <x:v>90</x:v>
@@ -3223,7 +2242,7 @@
     </x:row>
     <x:row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <x:c r="A51" s="1" t="s">
-        <x:v>445</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="B51" s="1" t="s">
         <x:v>128</x:v>
@@ -3235,9 +2254,9 @@
         <x:v>128</x:v>
       </x:c>
     </x:row>
-    <x:row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A52" s="1" t="s">
-        <x:v>446</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B52" s="1" t="s">
         <x:v>91</x:v>
@@ -3249,9 +2268,9 @@
         <x:v>91</x:v>
       </x:c>
     </x:row>
-    <x:row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A53" s="1" t="s">
-        <x:v>447</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B53" s="1" t="s">
         <x:v>92</x:v>
@@ -3263,9 +2282,9 @@
         <x:v>92</x:v>
       </x:c>
     </x:row>
-    <x:row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A54" s="1" t="s">
-        <x:v>448</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B54" s="1" t="s">
         <x:v>93</x:v>
@@ -3277,9 +2296,9 @@
         <x:v>93</x:v>
       </x:c>
     </x:row>
-    <x:row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A55" s="1" t="s">
-        <x:v>449</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B55" s="1" t="s">
         <x:v>94</x:v>
@@ -3291,9 +2310,9 @@
         <x:v>94</x:v>
       </x:c>
     </x:row>
-    <x:row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A56" s="1" t="s">
-        <x:v>450</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B56" s="1" t="s">
         <x:v>95</x:v>
@@ -3305,9 +2324,9 @@
         <x:v>95</x:v>
       </x:c>
     </x:row>
-    <x:row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A57" s="1" t="s">
-        <x:v>451</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="B57" s="1" t="s">
         <x:v>96</x:v>
@@ -3319,9 +2338,9 @@
         <x:v>96</x:v>
       </x:c>
     </x:row>
-    <x:row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A58" s="1" t="s">
-        <x:v>452</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B58" s="1" t="s">
         <x:v>97</x:v>
@@ -3333,9 +2352,9 @@
         <x:v>97</x:v>
       </x:c>
     </x:row>
-    <x:row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A59" s="1" t="s">
-        <x:v>453</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B59" s="1" t="s">
         <x:v>98</x:v>
@@ -3347,9 +2366,9 @@
         <x:v>98</x:v>
       </x:c>
     </x:row>
-    <x:row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A60" s="1" t="s">
-        <x:v>454</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="B60" s="1" t="s">
         <x:v>99</x:v>
@@ -3361,9 +2380,9 @@
         <x:v>99</x:v>
       </x:c>
     </x:row>
-    <x:row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A61" s="1" t="s">
-        <x:v>455</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="B61" s="1" t="s">
         <x:v>100</x:v>
@@ -3375,9 +2394,9 @@
         <x:v>100</x:v>
       </x:c>
     </x:row>
-    <x:row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A62" s="1" t="s">
-        <x:v>456</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B62" s="1" t="s">
         <x:v>101</x:v>
@@ -3389,9 +2408,9 @@
         <x:v>101</x:v>
       </x:c>
     </x:row>
-    <x:row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A63" s="1" t="s">
-        <x:v>457</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="B63" s="1" t="s">
         <x:v>45</x:v>
@@ -3403,9 +2422,9 @@
         <x:v>112</x:v>
       </x:c>
     </x:row>
-    <x:row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A64" s="1" t="s">
-        <x:v>458</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="B64" s="1" t="s">
         <x:v>102</x:v>
@@ -3417,9 +2436,9 @@
         <x:v>113</x:v>
       </x:c>
     </x:row>
-    <x:row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A65" s="1" t="s">
-        <x:v>459</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="B65" s="1" t="s">
         <x:v>103</x:v>
@@ -3431,9 +2450,9 @@
         <x:v>114</x:v>
       </x:c>
     </x:row>
-    <x:row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A66" s="1" t="s">
-        <x:v>460</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="B66" s="1" t="s">
         <x:v>60</x:v>
@@ -3445,9 +2464,9 @@
         <x:v>60</x:v>
       </x:c>
     </x:row>
-    <x:row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A67" s="1" t="s">
-        <x:v>461</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="B67" s="1" t="s">
         <x:v>104</x:v>
@@ -3459,9 +2478,9 @@
         <x:v>115</x:v>
       </x:c>
     </x:row>
-    <x:row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A68" s="1" t="s">
-        <x:v>462</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="B68" s="1" t="s">
         <x:v>55</x:v>
@@ -3473,9 +2492,9 @@
         <x:v>116</x:v>
       </x:c>
     </x:row>
-    <x:row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A69" s="1" t="s">
-        <x:v>463</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B69" s="1" t="s">
         <x:v>57</x:v>
@@ -3487,9 +2506,9 @@
         <x:v>117</x:v>
       </x:c>
     </x:row>
-    <x:row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <x:row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A70" s="1" t="s">
-        <x:v>464</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="B70" s="1" t="s">
         <x:v>105</x:v>

</xml_diff>

<commit_message>
fix empty lines in localized docs
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -704,6 +704,67 @@
   </x:si>
   <x:si>
     <x:t>ВВОД</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">@printer Fullscreen
+{0}[i]{1}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">{0}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">@spawn Rain wait:false
+{0}[br][i]{1}[spawn ShakePrinter params:,1 wait:false]{2}[skipInput]
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+# TestLabel
+@resetText
+; Test comment.
+@printer Wide time:0
+k: {0}[i]{1}[br 2]{2}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">@print {0} speed:0.5 default:false
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">@char Kohaku pos:10,50,-1
+@choice {0} pos:10,50
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">@stop
+@despawn Rain wait:false
+y.Default: {0}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+@goto Script002</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"># Start
+{0}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+@input i summary:{0} value:{1}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">@stop
+{0}
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">
+@goto .Start</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">@printer Fullscreen
@@ -1197,7 +1258,7 @@
     </x:row>
     <x:row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>229</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>3</x:v>
@@ -1225,7 +1286,7 @@
     </x:row>
     <x:row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <x:c r="A4" s="1" t="s">
-        <x:v>230</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
         <x:v>4</x:v>
@@ -1239,7 +1300,7 @@
     </x:row>
     <x:row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>231</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
         <x:v>5</x:v>
@@ -1281,7 +1342,7 @@
     </x:row>
     <x:row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <x:c r="A8" s="1" t="s">
-        <x:v>232</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
         <x:v>6</x:v>
@@ -1323,7 +1384,7 @@
     </x:row>
     <x:row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A11" s="1" t="s">
-        <x:v>233</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
         <x:v>7</x:v>
@@ -1337,7 +1398,7 @@
     </x:row>
     <x:row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A12" s="1" t="s">
-        <x:v>234</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>8</x:v>
@@ -1351,7 +1412,7 @@
     </x:row>
     <x:row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
-        <x:v>235</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
         <x:v>129</x:v>
@@ -1365,7 +1426,7 @@
     </x:row>
     <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A14" s="1" t="s">
-        <x:v>236</x:v>
+        <x:v>248</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1403,7 +1464,7 @@
     </x:row>
     <x:row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>237</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
         <x:v>29</x:v>
@@ -1417,7 +1478,7 @@
     </x:row>
     <x:row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
-        <x:v>238</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>30</x:v>
@@ -1445,7 +1506,7 @@
     </x:row>
     <x:row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>239</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
         <x:v>32</x:v>
@@ -1459,7 +1520,7 @@
     </x:row>
     <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <x:c r="A6" s="1" t="s">
-        <x:v>240</x:v>
+        <x:v>252</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
add script value example
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elringus\Documents\UnityProjects\Naninovel\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFA7997-2195-48C0-A02B-FCCF6B34F78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AFEF55-6465-44DF-B950-0C7E8725C1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="465" windowWidth="29430" windowHeight="20130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13140" yWindow="1515" windowWidth="24675" windowHeight="18930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts&gt;Script001" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Scripts&gt;Subfolder&gt;Script003" sheetId="6" r:id="rId3"/>
     <sheet name="Text&gt;CharacterNames" sheetId="4" r:id="rId4"/>
     <sheet name="Text&gt;DefaultUI" sheetId="5" r:id="rId5"/>
+    <sheet name="Text&gt;Script" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="256">
   <si>
     <t>Template</t>
   </si>
@@ -707,6 +708,39 @@
   </si>
   <si>
     <t>サブフォルダーでスクリプトをテストします。</t>
+  </si>
+  <si>
+    <t>"Lorem ipsum"</t>
+  </si>
+  <si>
+    <t>"Реликтовый ледник"</t>
+  </si>
+  <si>
+    <t>遺物氷河</t>
+  </si>
+  <si>
+    <t>t_Foo: {0}</t>
+  </si>
+  <si>
+    <t>t_Bar: {0}</t>
+  </si>
+  <si>
+    <t>Foo</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>ふぉお</t>
+  </si>
+  <si>
+    <t>Фу</t>
+  </si>
+  <si>
+    <t>ばら</t>
+  </si>
+  <si>
+    <t>Бар</t>
   </si>
   <si>
     <t xml:space="preserve">@printer Fullscreen
@@ -756,10 +790,15 @@
   </si>
   <si>
     <t xml:space="preserve">
+{0}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 @goto Script002</t>
   </si>
   <si>
-    <t>"Lorem ipsum"</t>
+    <t>Value of t_Foo: {t_Foo}, value of t_Bar: {t_Bar}.</t>
   </si>
   <si>
     <t xml:space="preserve"># Start
@@ -786,10 +825,10 @@
 </t>
   </si>
   <si>
-    <t>"Реликтовый ледник"</t>
-  </si>
-  <si>
-    <t>遺物氷河</t>
+    <t>Значение t_Foo: {t_Foo}, значениеf t_Bar: {t_Bar}.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t_Foo の値: {t_Foo},  t_Bar の値: {t_Bar}.</t>
   </si>
 </sst>
 </file>
@@ -1140,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B14E23-E089-464E-BEA1-58428DA8F9CD}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1206,7 @@
     </row>
     <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>207</v>
@@ -1195,7 +1234,7 @@
     </row>
     <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1209,7 +1248,7 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -1251,7 +1290,7 @@
     </row>
     <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -1293,7 +1332,7 @@
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -1307,35 +1346,35 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>198</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1349,7 +1388,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B15" t="s">
         <v>123</v>
@@ -1363,7 +1402,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>235</v>
+        <v>246</v>
+      </c>
+      <c r="B16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +1454,7 @@
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>26</v>
@@ -1415,7 +1468,7 @@
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
@@ -1443,7 +1496,7 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>199</v>
@@ -1457,7 +1510,7 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1498,7 +1551,7 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>223</v>
@@ -2579,4 +2632,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>